<commit_message>
finish menu and home
</commit_message>
<xml_diff>
--- a/Mobi/Mobi/Support/Resource/Data/ap sim so.xlsx
+++ b/Mobi/Mobi/Support/Resource/Data/ap sim so.xlsx
@@ -1,13 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HeoConUnIn/Desktop/Working/Toan/Mobi/Mobi/Support/Resource/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="1100" yWindow="440" windowWidth="27700" windowHeight="17560" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Trang tính1" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="bugs" sheetId="2" r:id="rId4"/>
+    <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
+    <sheet name="bugs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -298,45 +314,80 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -349,6 +400,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -363,6 +415,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -373,6 +426,7 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -385,476 +439,738 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
+    <cellStyle name="Accent2" xfId="1" builtinId="33"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="46.57"/>
-    <col customWidth="1" min="2" max="2" width="27.71"/>
-    <col customWidth="1" min="3" max="3" width="57.86"/>
-    <col customWidth="1" min="4" max="4" width="40.71"/>
-    <col customWidth="1" min="5" max="5" width="22.71"/>
+    <col min="1" max="1" width="46.5" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="57.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17"/>
+      <c r="B3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="7"/>
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="17"/>
+      <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
+      <c r="B5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="8"/>
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
+      <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7">
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8">
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="5" t="s">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14">
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" s="9" t="s">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" s="9" t="s">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="7"/>
-      <c r="B19" s="5" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="9"/>
+      <c r="B19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="6" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="7"/>
-      <c r="B20" s="5" t="s">
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="9"/>
+      <c r="B20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="7"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="5" t="s">
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="9"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="7"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="7"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="7"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="7"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="7"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="7"/>
-    </row>
-    <row r="29">
-      <c r="B29" s="12" t="s">
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="9"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="9"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="9"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="9"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="9"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="3" t="s">
+    </row>
+    <row r="31" spans="1:5" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
+    <row r="32" spans="1:5" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12"/>
+      <c r="C32" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
+    <row r="33" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="3"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="s">
+    <row r="36" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="1" t="s">
+    <row r="39" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:3" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="15" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>68</v>
       </c>
@@ -865,22 +1181,22 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
         <v>74</v>
       </c>
@@ -888,22 +1204,22 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>79</v>
       </c>
@@ -914,7 +1230,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
         <v>76</v>
       </c>
@@ -922,12 +1238,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
         <v>83</v>
       </c>
@@ -939,48 +1255,49 @@
     <mergeCell ref="A18:A28"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B1"/>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="C3"/>
-    <hyperlink r:id="rId4" ref="C4"/>
-    <hyperlink r:id="rId5" ref="C5"/>
-    <hyperlink r:id="rId6" ref="B6"/>
-    <hyperlink r:id="rId7" ref="C7"/>
-    <hyperlink r:id="rId8" ref="C8"/>
-    <hyperlink r:id="rId9" ref="C9"/>
-    <hyperlink r:id="rId10" ref="C11"/>
-    <hyperlink r:id="rId11" ref="C12"/>
-    <hyperlink r:id="rId12" ref="C13"/>
-    <hyperlink r:id="rId13" ref="C14"/>
-    <hyperlink r:id="rId14" ref="C15"/>
-    <hyperlink r:id="rId15" ref="C16"/>
-    <hyperlink r:id="rId16" ref="D19"/>
-    <hyperlink r:id="rId17" ref="D20"/>
-    <hyperlink r:id="rId18" ref="D21"/>
-    <hyperlink r:id="rId19" ref="B31"/>
-    <hyperlink r:id="rId20" ref="D31"/>
-    <hyperlink r:id="rId21" ref="B35"/>
-    <hyperlink r:id="rId22" ref="B38"/>
-    <hyperlink r:id="rId23" ref="B40"/>
-    <hyperlink r:id="rId24" ref="B43"/>
-    <hyperlink r:id="rId25" ref="B45"/>
-    <hyperlink r:id="rId26" ref="B49"/>
-    <hyperlink r:id="rId27" ref="B54"/>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
+    <hyperlink ref="C7" r:id="rId7"/>
+    <hyperlink ref="C8" r:id="rId8"/>
+    <hyperlink ref="C9" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="D19" r:id="rId16"/>
+    <hyperlink ref="D20" r:id="rId17"/>
+    <hyperlink ref="D21" r:id="rId18"/>
+    <hyperlink ref="B31" r:id="rId19"/>
+    <hyperlink ref="D31" r:id="rId20"/>
+    <hyperlink ref="B35" r:id="rId21"/>
+    <hyperlink ref="B38" r:id="rId22"/>
+    <hyperlink ref="B40" r:id="rId23"/>
+    <hyperlink ref="B43" r:id="rId24"/>
+    <hyperlink ref="B45" r:id="rId25"/>
+    <hyperlink ref="B49" r:id="rId26"/>
+    <hyperlink ref="B54" r:id="rId27"/>
   </hyperlinks>
-  <drawing r:id="rId28"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish projec +  send file
</commit_message>
<xml_diff>
--- a/Mobi/Mobi/Support/Resource/Data/ap sim so.xlsx
+++ b/Mobi/Mobi/Support/Resource/Data/ap sim so.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HeoConUnIn/Desktop/Working/Toan/Mobi/Mobi/Support/Resource/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HeoConUnIn/Desktop/Working/Mobifone_IOS/Mobi/Mobi/Support/Resource/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -315,11 +315,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -361,6 +368,10 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -381,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -430,19 +441,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -459,30 +457,33 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
@@ -767,249 +768,247 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="46.5" customWidth="1"/>
+    <col min="1" max="1" width="109" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="57.83203125" customWidth="1"/>
     <col min="4" max="4" width="40.6640625" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:7" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
-      <c r="B4" s="15" t="s">
+    <row r="4" spans="1:7" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="15" t="s">
+    <row r="5" spans="1:7" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="15" t="s">
+    <row r="6" spans="1:7" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13"/>
+      <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="13" t="s">
+    <row r="7" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
-      <c r="B8" s="6" t="s">
+    </row>
+    <row r="8" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="6" t="s">
+    <row r="15" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="6" t="s">
+    <row r="16" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="9"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="7"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="9"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="4" t="s">
         <v>44</v>
       </c>
@@ -1019,133 +1018,133 @@
       <c r="D20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="9"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="9"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="9"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="9"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="9"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="9"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="9"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="8" t="s">
+      <c r="A27" s="15"/>
+    </row>
+    <row r="28" spans="1:5" ht="106" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="15"/>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B29" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="12" t="s">
+    <row r="31" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
-      <c r="C32" s="11" t="s">
+    <row r="32" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="14"/>
+      <c r="C32" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
+    <row r="33" spans="1:3" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:3" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
+    <row r="35" spans="1:3" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
+    <row r="36" spans="1:3" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:3" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
+    <row r="39" spans="1:3" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:3" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
+    <row r="41" spans="1:3" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1154,14 +1153,14 @@
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="15" t="s">
+    <row r="43" spans="1:3" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="10" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1219,40 +1218,41 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:3" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:3" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:3" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:3" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="9" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A18:A28"/>
+    <mergeCell ref="A55:A56"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix: 	+ Not show word in from register 	+ Upload image 	+ Lost tap bar after that chosse image
</commit_message>
<xml_diff>
--- a/Mobi/Mobi/Support/Resource/Data/ap sim so.xlsx
+++ b/Mobi/Mobi/Support/Resource/Data/ap sim so.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HeoConUnIn/Desktop/Working/Mobifone_IOS/Mobi/Mobi/Support/Resource/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/DeskTop/Working/Mobifone_IOS/Mobi/Mobi/Support/Resource/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="440" windowWidth="27700" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="440" windowWidth="27680" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -480,10 +480,10 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
@@ -768,7 +768,7 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:A28"/>
     </sheetView>
   </sheetViews>
@@ -986,7 +986,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="15" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -997,7 +997,7 @@
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="15"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="4" t="s">
         <v>42</v>
       </c>
@@ -1008,7 +1008,7 @@
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="15"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="4" t="s">
         <v>44</v>
       </c>
@@ -1021,7 +1021,7 @@
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="15"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="6"/>
       <c r="C21" s="4" t="s">
         <v>47</v>
@@ -1032,45 +1032,45 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="15"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="15"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="15"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="15"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="15"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="15"/>
+      <c r="A27" s="16"/>
     </row>
     <row r="28" spans="1:5" ht="106" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="15"/>
+      <c r="A28" s="16"/>
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">

</xml_diff>